<commit_message>
add analysis for korea Signed-off-by: jxstar <13911191965@139.com>
</commit_message>
<xml_diff>
--- a/japan.tourists.number.xlsx
+++ b/japan.tourists.number.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" iterate="1" iterateCount="1000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="26">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,16 +101,25 @@
   <si>
     <t>2017</t>
   </si>
+  <si>
+    <t>taiwan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>korea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +172,12 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -204,7 +219,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -220,6 +235,7 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma 2" xfId="3"/>
@@ -527,15 +543,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H182"/>
+  <dimension ref="A1:J182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="F154" sqref="F154:F157"/>
+    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
+      <selection activeCell="N146" sqref="N146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="9" max="10" width="8.875" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -560,8 +579,14 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1">
         <v>37257</v>
       </c>
@@ -581,7 +606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3" s="1">
         <v>37288</v>
       </c>
@@ -601,7 +626,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:10">
       <c r="A4" s="1">
         <v>37316</v>
       </c>
@@ -621,7 +646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:10">
       <c r="A5" s="1">
         <v>37347</v>
       </c>
@@ -641,7 +666,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:10">
       <c r="A6" s="1">
         <v>37377</v>
       </c>
@@ -661,7 +686,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:10">
       <c r="A7" s="1">
         <v>37408</v>
       </c>
@@ -681,7 +706,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:10">
       <c r="A8" s="1">
         <v>37438</v>
       </c>
@@ -701,7 +726,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:10">
       <c r="A9" s="1">
         <v>37469</v>
       </c>
@@ -721,7 +746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:10">
       <c r="A10" s="1">
         <v>37500</v>
       </c>
@@ -741,7 +766,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:10">
       <c r="A11" s="1">
         <v>37530</v>
       </c>
@@ -761,7 +786,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:10">
       <c r="A12" s="1">
         <v>37561</v>
       </c>
@@ -781,7 +806,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:10">
       <c r="A13" s="1">
         <v>37591</v>
       </c>
@@ -801,7 +826,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:10">
       <c r="A14" s="1">
         <v>37622</v>
       </c>
@@ -821,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:10">
       <c r="A15" s="1">
         <v>37653</v>
       </c>
@@ -841,7 +866,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:10">
       <c r="A16" s="1">
         <v>37681</v>
       </c>
@@ -1821,7 +1846,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:10">
       <c r="A65" s="1">
         <v>39173</v>
       </c>
@@ -1841,7 +1866,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:10">
       <c r="A66" s="1">
         <v>39203</v>
       </c>
@@ -1861,7 +1886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:10">
       <c r="A67" s="1">
         <v>39234</v>
       </c>
@@ -1881,7 +1906,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:10">
       <c r="A68" s="1">
         <v>39264</v>
       </c>
@@ -1901,7 +1926,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:10">
       <c r="A69" s="1">
         <v>39295</v>
       </c>
@@ -1921,7 +1946,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:10">
       <c r="A70" s="1">
         <v>39326</v>
       </c>
@@ -1941,7 +1966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:10">
       <c r="A71" s="1">
         <v>39356</v>
       </c>
@@ -1961,7 +1986,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:10">
       <c r="A72" s="1">
         <v>39387</v>
       </c>
@@ -1981,7 +2006,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:10">
       <c r="A73" s="1">
         <v>39417</v>
       </c>
@@ -2001,7 +2026,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:10">
       <c r="A74" s="1">
         <v>39448</v>
       </c>
@@ -2021,7 +2046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:10">
       <c r="A75" s="1">
         <v>39479</v>
       </c>
@@ -2041,7 +2066,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:10">
       <c r="A76" s="1">
         <v>39508</v>
       </c>
@@ -2061,7 +2086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:10">
       <c r="A77" s="1">
         <v>39539</v>
       </c>
@@ -2081,7 +2106,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:10">
       <c r="A78" s="1">
         <v>39569</v>
       </c>
@@ -2101,7 +2126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:10">
       <c r="A79" s="1">
         <v>39600</v>
       </c>
@@ -2121,7 +2146,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:10">
       <c r="A80" s="1">
         <v>39630</v>
       </c>
@@ -2140,8 +2165,14 @@
       <c r="H80">
         <v>7</v>
       </c>
-    </row>
-    <row r="81" spans="1:8">
+      <c r="I80" s="2">
+        <v>30323</v>
+      </c>
+      <c r="J80" s="2">
+        <v>101061</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81" s="1">
         <v>39661</v>
       </c>
@@ -2160,8 +2191,14 @@
       <c r="H81">
         <v>8</v>
       </c>
-    </row>
-    <row r="82" spans="1:8">
+      <c r="I81" s="2">
+        <v>29281</v>
+      </c>
+      <c r="J81" s="2">
+        <v>115042</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82" s="1">
         <v>39692</v>
       </c>
@@ -2180,8 +2217,14 @@
       <c r="H82">
         <v>9</v>
       </c>
-    </row>
-    <row r="83" spans="1:8">
+      <c r="I82" s="2">
+        <v>33251</v>
+      </c>
+      <c r="J82" s="2">
+        <v>112988</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83" s="1">
         <v>39722</v>
       </c>
@@ -2200,8 +2243,14 @@
       <c r="H83">
         <v>10</v>
       </c>
-    </row>
-    <row r="84" spans="1:8">
+      <c r="I83" s="2">
+        <v>34780</v>
+      </c>
+      <c r="J83" s="2">
+        <v>104710</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84" s="1">
         <v>39753</v>
       </c>
@@ -2220,8 +2269,14 @@
       <c r="H84">
         <v>11</v>
       </c>
-    </row>
-    <row r="85" spans="1:8">
+      <c r="I84" s="2">
+        <v>35238</v>
+      </c>
+      <c r="J84" s="2">
+        <v>88916</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85" s="1">
         <v>39783</v>
       </c>
@@ -2240,8 +2295,14 @@
       <c r="H85">
         <v>12</v>
       </c>
-    </row>
-    <row r="86" spans="1:8">
+      <c r="I85" s="2">
+        <v>35114</v>
+      </c>
+      <c r="J85" s="2">
+        <v>85921</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86" s="1">
         <v>39814</v>
       </c>
@@ -2260,8 +2321,14 @@
       <c r="H86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:8">
+      <c r="I86" s="2">
+        <v>43995</v>
+      </c>
+      <c r="J86" s="2">
+        <v>93007</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87" s="1">
         <v>39845</v>
       </c>
@@ -2280,8 +2347,14 @@
       <c r="H87">
         <v>2</v>
       </c>
-    </row>
-    <row r="88" spans="1:8">
+      <c r="I87" s="2">
+        <v>42248</v>
+      </c>
+      <c r="J87" s="2">
+        <v>127979</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88" s="1">
         <v>39873</v>
       </c>
@@ -2300,8 +2373,14 @@
       <c r="H88">
         <v>3</v>
       </c>
-    </row>
-    <row r="89" spans="1:8">
+      <c r="I88" s="2">
+        <v>87002</v>
+      </c>
+      <c r="J88" s="2">
+        <v>111915</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89" s="1">
         <v>39904</v>
       </c>
@@ -2320,8 +2399,14 @@
       <c r="H89">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:8">
+      <c r="I89" s="2">
+        <v>131464</v>
+      </c>
+      <c r="J89" s="2">
+        <v>107872</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90" s="1">
         <v>39934</v>
       </c>
@@ -2340,8 +2425,14 @@
       <c r="H90">
         <v>5</v>
       </c>
-    </row>
-    <row r="91" spans="1:8">
+      <c r="I90" s="2">
+        <v>110244</v>
+      </c>
+      <c r="J90" s="2">
+        <v>86392</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91" s="1">
         <v>39965</v>
       </c>
@@ -2360,8 +2451,14 @@
       <c r="H91">
         <v>6</v>
       </c>
-    </row>
-    <row r="92" spans="1:8">
+      <c r="I91" s="2">
+        <v>57472</v>
+      </c>
+      <c r="J91" s="2">
+        <v>77830</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92" s="1">
         <v>39995</v>
       </c>
@@ -2380,8 +2477,14 @@
       <c r="H92">
         <v>7</v>
       </c>
-    </row>
-    <row r="93" spans="1:8">
+      <c r="I92" s="2">
+        <v>70157</v>
+      </c>
+      <c r="J92" s="2">
+        <v>107490</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93" s="1">
         <v>40026</v>
       </c>
@@ -2400,8 +2503,14 @@
       <c r="H93">
         <v>8</v>
       </c>
-    </row>
-    <row r="94" spans="1:8">
+      <c r="I93" s="2">
+        <v>80883</v>
+      </c>
+      <c r="J93" s="2">
+        <v>160424</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94" s="1">
         <v>40057</v>
       </c>
@@ -2420,8 +2529,14 @@
       <c r="H94">
         <v>9</v>
       </c>
-    </row>
-    <row r="95" spans="1:8">
+      <c r="I94" s="2">
+        <v>64386</v>
+      </c>
+      <c r="J94" s="2">
+        <v>126793</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95" s="1">
         <v>40087</v>
       </c>
@@ -2440,8 +2555,14 @@
       <c r="H95">
         <v>10</v>
       </c>
-    </row>
-    <row r="96" spans="1:8">
+      <c r="I95" s="2">
+        <v>78175</v>
+      </c>
+      <c r="J95" s="2">
+        <v>138898</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96" s="1">
         <v>40118</v>
       </c>
@@ -2460,8 +2581,14 @@
       <c r="H96">
         <v>11</v>
       </c>
-    </row>
-    <row r="97" spans="1:8">
+      <c r="I96" s="2">
+        <v>113807</v>
+      </c>
+      <c r="J96" s="2">
+        <v>102329</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97" s="1">
         <v>40148</v>
       </c>
@@ -2480,8 +2607,14 @@
       <c r="H97">
         <v>12</v>
       </c>
-    </row>
-    <row r="98" spans="1:8">
+      <c r="I97" s="2">
+        <v>92290</v>
+      </c>
+      <c r="J97" s="2">
+        <v>101388</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98" s="1">
         <v>40179</v>
       </c>
@@ -2500,8 +2633,14 @@
       <c r="H98">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:8">
+      <c r="I98" s="2">
+        <v>86891</v>
+      </c>
+      <c r="J98" s="2">
+        <v>91252</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99" s="1">
         <v>40210</v>
       </c>
@@ -2520,8 +2659,14 @@
       <c r="H99">
         <v>2</v>
       </c>
-    </row>
-    <row r="100" spans="1:8">
+      <c r="I99" s="2">
+        <v>107628</v>
+      </c>
+      <c r="J99" s="2">
+        <v>140571</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100" s="1">
         <v>40238</v>
       </c>
@@ -2540,8 +2685,14 @@
       <c r="H100">
         <v>3</v>
       </c>
-    </row>
-    <row r="101" spans="1:8">
+      <c r="I100" s="2">
+        <v>149617</v>
+      </c>
+      <c r="J100" s="2">
+        <v>141457</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101" s="1">
         <v>40269</v>
       </c>
@@ -2560,8 +2711,14 @@
       <c r="H101">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:8">
+      <c r="I101" s="2">
+        <v>180915</v>
+      </c>
+      <c r="J101" s="2">
+        <v>147680</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10">
       <c r="A102" s="1">
         <v>40299</v>
       </c>
@@ -2580,8 +2737,14 @@
       <c r="H102">
         <v>5</v>
       </c>
-    </row>
-    <row r="103" spans="1:8">
+      <c r="I102" s="2">
+        <v>179394</v>
+      </c>
+      <c r="J102" s="2">
+        <v>154066</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10">
       <c r="A103" s="1">
         <v>40330</v>
       </c>
@@ -2600,8 +2763,14 @@
       <c r="H103">
         <v>6</v>
       </c>
-    </row>
-    <row r="104" spans="1:8">
+      <c r="I103" s="2">
+        <v>135603</v>
+      </c>
+      <c r="J103" s="2">
+        <v>150119</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10">
       <c r="A104" s="1">
         <v>40360</v>
       </c>
@@ -2620,8 +2789,14 @@
       <c r="H104">
         <v>7</v>
       </c>
-    </row>
-    <row r="105" spans="1:8">
+      <c r="I104" s="2">
+        <v>129160</v>
+      </c>
+      <c r="J104" s="2">
+        <v>195188</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10">
       <c r="A105" s="1">
         <v>40391</v>
       </c>
@@ -2640,8 +2815,14 @@
       <c r="H105">
         <v>8</v>
       </c>
-    </row>
-    <row r="106" spans="1:8">
+      <c r="I105" s="2">
+        <v>118616</v>
+      </c>
+      <c r="J105" s="2">
+        <v>241987</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10">
       <c r="A106" s="1">
         <v>40422</v>
       </c>
@@ -2660,8 +2841,14 @@
       <c r="H106">
         <v>9</v>
       </c>
-    </row>
-    <row r="107" spans="1:8">
+      <c r="I106" s="2">
+        <v>105707</v>
+      </c>
+      <c r="J106" s="2">
+        <v>176196</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10">
       <c r="A107" s="1">
         <v>40452</v>
       </c>
@@ -2680,8 +2867,14 @@
       <c r="H107">
         <v>10</v>
       </c>
-    </row>
-    <row r="108" spans="1:8">
+      <c r="I107" s="2">
+        <v>150221</v>
+      </c>
+      <c r="J107" s="2">
+        <v>181428</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10">
       <c r="A108" s="1">
         <v>40483</v>
       </c>
@@ -2700,8 +2893,14 @@
       <c r="H108">
         <v>11</v>
       </c>
-    </row>
-    <row r="109" spans="1:8">
+      <c r="I108" s="2">
+        <v>165065</v>
+      </c>
+      <c r="J108" s="2">
+        <v>136152</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10">
       <c r="A109" s="1">
         <v>40513</v>
       </c>
@@ -2720,8 +2919,14 @@
       <c r="H109">
         <v>12</v>
       </c>
-    </row>
-    <row r="110" spans="1:8">
+      <c r="I109" s="2">
+        <v>121918</v>
+      </c>
+      <c r="J109" s="2">
+        <v>119061</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10">
       <c r="A110" s="1">
         <v>40544</v>
       </c>
@@ -2740,8 +2945,14 @@
       <c r="H110">
         <v>1</v>
       </c>
-    </row>
-    <row r="111" spans="1:8">
+      <c r="I110" s="2">
+        <v>101354</v>
+      </c>
+      <c r="J110" s="2">
+        <v>113927</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10">
       <c r="A111" s="1">
         <v>40575</v>
       </c>
@@ -2760,8 +2971,14 @@
       <c r="H111">
         <v>2</v>
       </c>
-    </row>
-    <row r="112" spans="1:8">
+      <c r="I111" s="2">
+        <v>115845</v>
+      </c>
+      <c r="J111" s="2">
+        <v>157019</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10">
       <c r="A112" s="1">
         <v>40603</v>
       </c>
@@ -2780,8 +2997,14 @@
       <c r="H112">
         <v>3</v>
       </c>
-    </row>
-    <row r="113" spans="1:8">
+      <c r="I112" s="2">
+        <v>153649</v>
+      </c>
+      <c r="J112" s="2">
+        <v>163261</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10">
       <c r="A113" s="1">
         <v>40634</v>
       </c>
@@ -2800,8 +3023,14 @@
       <c r="H113">
         <v>4</v>
       </c>
-    </row>
-    <row r="114" spans="1:8">
+      <c r="I113" s="2">
+        <v>193457</v>
+      </c>
+      <c r="J113" s="2">
+        <v>153875</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10">
       <c r="A114" s="1">
         <v>40664</v>
       </c>
@@ -2820,8 +3049,14 @@
       <c r="H114">
         <v>5</v>
       </c>
-    </row>
-    <row r="115" spans="1:8">
+      <c r="I114" s="2">
+        <v>150479</v>
+      </c>
+      <c r="J114" s="2">
+        <v>152347</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10">
       <c r="A115" s="1">
         <v>40695</v>
       </c>
@@ -2840,8 +3075,14 @@
       <c r="H115">
         <v>6</v>
       </c>
-    </row>
-    <row r="116" spans="1:8">
+      <c r="I115" s="2">
+        <v>114435</v>
+      </c>
+      <c r="J115" s="2">
+        <v>179508</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10">
       <c r="A116" s="1">
         <v>40725</v>
       </c>
@@ -2860,8 +3101,14 @@
       <c r="H116">
         <v>7</v>
       </c>
-    </row>
-    <row r="117" spans="1:8">
+      <c r="I116" s="2">
+        <v>135968</v>
+      </c>
+      <c r="J116" s="2">
+        <v>244573</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10">
       <c r="A117" s="1">
         <v>40756</v>
       </c>
@@ -2880,8 +3127,14 @@
       <c r="H117">
         <v>8</v>
       </c>
-    </row>
-    <row r="118" spans="1:8">
+      <c r="I117" s="2">
+        <v>138673</v>
+      </c>
+      <c r="J117" s="2">
+        <v>276299</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10">
       <c r="A118" s="1">
         <v>40787</v>
       </c>
@@ -2900,8 +3153,14 @@
       <c r="H118">
         <v>9</v>
       </c>
-    </row>
-    <row r="119" spans="1:8">
+      <c r="I118" s="2">
+        <v>122574</v>
+      </c>
+      <c r="J118" s="2">
+        <v>231462</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10">
       <c r="A119" s="1">
         <v>40817</v>
       </c>
@@ -2920,8 +3179,14 @@
       <c r="H119">
         <v>10</v>
       </c>
-    </row>
-    <row r="120" spans="1:8">
+      <c r="I119" s="2">
+        <v>163290</v>
+      </c>
+      <c r="J119" s="2">
+        <v>214681</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10">
       <c r="A120" s="1">
         <v>40848</v>
       </c>
@@ -2940,8 +3205,14 @@
       <c r="H120">
         <v>11</v>
       </c>
-    </row>
-    <row r="121" spans="1:8">
+      <c r="I120" s="2">
+        <v>213144</v>
+      </c>
+      <c r="J120" s="2">
+        <v>174164</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10">
       <c r="A121" s="1">
         <v>40878</v>
       </c>
@@ -2960,8 +3231,14 @@
       <c r="H121">
         <v>12</v>
       </c>
-    </row>
-    <row r="122" spans="1:8">
+      <c r="I121" s="2">
+        <v>181317</v>
+      </c>
+      <c r="J121" s="2">
+        <v>159080</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10">
       <c r="A122" s="1">
         <v>40909</v>
       </c>
@@ -2980,8 +3257,14 @@
       <c r="H122">
         <v>1</v>
       </c>
-    </row>
-    <row r="123" spans="1:8">
+      <c r="I122" s="2">
+        <v>140432</v>
+      </c>
+      <c r="J122" s="2">
+        <v>167022</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10">
       <c r="A123" s="1">
         <v>40940</v>
       </c>
@@ -3000,8 +3283,14 @@
       <c r="H123">
         <v>2</v>
       </c>
-    </row>
-    <row r="124" spans="1:8">
+      <c r="I123" s="2">
+        <v>163442</v>
+      </c>
+      <c r="J123" s="2">
+        <v>173790</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10">
       <c r="A124" s="1">
         <v>40969</v>
       </c>
@@ -3020,8 +3309,14 @@
       <c r="H124">
         <v>3</v>
       </c>
-    </row>
-    <row r="125" spans="1:8">
+      <c r="I124" s="2">
+        <v>253205</v>
+      </c>
+      <c r="J124" s="2">
+        <v>183691</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10">
       <c r="A125" s="1">
         <v>41000</v>
       </c>
@@ -3040,8 +3335,14 @@
       <c r="H125">
         <v>4</v>
       </c>
-    </row>
-    <row r="126" spans="1:8">
+      <c r="I125" s="2">
+        <v>278715</v>
+      </c>
+      <c r="J125" s="2">
+        <v>222114</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10">
       <c r="A126" s="1">
         <v>41030</v>
       </c>
@@ -3060,8 +3361,14 @@
       <c r="H126">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:8">
+      <c r="I126" s="2">
+        <v>228607</v>
+      </c>
+      <c r="J126" s="2">
+        <v>210439</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10">
       <c r="A127" s="1">
         <v>41061</v>
       </c>
@@ -3080,8 +3387,14 @@
       <c r="H127">
         <v>6</v>
       </c>
-    </row>
-    <row r="128" spans="1:8">
+      <c r="I127" s="2">
+        <v>199642</v>
+      </c>
+      <c r="J127" s="2">
+        <v>234482</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10">
       <c r="A128" s="1">
         <v>41091</v>
       </c>
@@ -3100,8 +3413,14 @@
       <c r="H128">
         <v>7</v>
       </c>
-    </row>
-    <row r="129" spans="1:8">
+      <c r="I128" s="2">
+        <v>235447</v>
+      </c>
+      <c r="J128" s="2">
+        <v>322917</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10">
       <c r="A129" s="1">
         <v>41122</v>
       </c>
@@ -3120,8 +3439,14 @@
       <c r="H129">
         <v>8</v>
       </c>
-    </row>
-    <row r="130" spans="1:8">
+      <c r="I129" s="2">
+        <v>205002</v>
+      </c>
+      <c r="J129" s="2">
+        <v>359065</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10">
       <c r="A130" s="1">
         <v>41153</v>
       </c>
@@ -3140,8 +3465,14 @@
       <c r="H130">
         <v>9</v>
       </c>
-    </row>
-    <row r="131" spans="1:8">
+      <c r="I130" s="2">
+        <v>185922</v>
+      </c>
+      <c r="J130" s="2">
+        <v>283402</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10">
       <c r="A131" s="1">
         <v>41183</v>
       </c>
@@ -3160,8 +3491,14 @@
       <c r="H131">
         <v>10</v>
       </c>
-    </row>
-    <row r="132" spans="1:8">
+      <c r="I131" s="2">
+        <v>224872</v>
+      </c>
+      <c r="J131" s="2">
+        <v>279440</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10">
       <c r="A132" s="1">
         <v>41214</v>
       </c>
@@ -3180,8 +3517,14 @@
       <c r="H132">
         <v>11</v>
       </c>
-    </row>
-    <row r="133" spans="1:8">
+      <c r="I132" s="2">
+        <v>242967</v>
+      </c>
+      <c r="J132" s="2">
+        <v>204533</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10">
       <c r="A133" s="1">
         <v>41244</v>
       </c>
@@ -3200,8 +3543,14 @@
       <c r="H133">
         <v>12</v>
       </c>
-    </row>
-    <row r="134" spans="1:8">
+      <c r="I133" s="2">
+        <v>228175</v>
+      </c>
+      <c r="J133" s="2">
+        <v>195997</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10">
       <c r="A134" s="1">
         <v>41275</v>
       </c>
@@ -3226,8 +3575,14 @@
       <c r="H134">
         <v>1</v>
       </c>
-    </row>
-    <row r="135" spans="1:8">
+      <c r="I134" s="2">
+        <v>195388</v>
+      </c>
+      <c r="J134" s="2">
+        <v>196371</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10">
       <c r="A135" s="1">
         <v>41306</v>
       </c>
@@ -3252,8 +3607,14 @@
       <c r="H135">
         <v>2</v>
       </c>
-    </row>
-    <row r="136" spans="1:8">
+      <c r="I135" s="2">
+        <v>216021</v>
+      </c>
+      <c r="J135" s="2">
+        <v>249698</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10">
       <c r="A136" s="1">
         <v>41334</v>
       </c>
@@ -3278,8 +3639,14 @@
       <c r="H136">
         <v>3</v>
       </c>
-    </row>
-    <row r="137" spans="1:8">
+      <c r="I136" s="2">
+        <v>269455</v>
+      </c>
+      <c r="J136" s="2">
+        <v>276479</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10">
       <c r="A137" s="1">
         <v>41365</v>
       </c>
@@ -3304,8 +3671,14 @@
       <c r="H137">
         <v>4</v>
       </c>
-    </row>
-    <row r="138" spans="1:8">
+      <c r="I137" s="2">
+        <v>298059</v>
+      </c>
+      <c r="J137" s="2">
+        <v>335069</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10">
       <c r="A138" s="1">
         <v>41395</v>
       </c>
@@ -3330,8 +3703,14 @@
       <c r="H138">
         <v>5</v>
       </c>
-    </row>
-    <row r="139" spans="1:8">
+      <c r="I138" s="2">
+        <v>217260</v>
+      </c>
+      <c r="J138" s="2">
+        <v>278723</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10">
       <c r="A139" s="1">
         <v>41426</v>
       </c>
@@ -3356,8 +3735,14 @@
       <c r="H139">
         <v>6</v>
       </c>
-    </row>
-    <row r="140" spans="1:8">
+      <c r="I139" s="2">
+        <v>220894</v>
+      </c>
+      <c r="J139" s="2">
+        <v>399031</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10">
       <c r="A140" s="1">
         <v>41456</v>
       </c>
@@ -3382,8 +3767,14 @@
       <c r="H140">
         <v>7</v>
       </c>
-    </row>
-    <row r="141" spans="1:8">
+      <c r="I140" s="2">
+        <v>248683</v>
+      </c>
+      <c r="J140" s="2">
+        <v>569787</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10">
       <c r="A141" s="1">
         <v>41487</v>
       </c>
@@ -3408,8 +3799,14 @@
       <c r="H141">
         <v>8</v>
       </c>
-    </row>
-    <row r="142" spans="1:8">
+      <c r="I141" s="2">
+        <v>240490</v>
+      </c>
+      <c r="J141" s="2">
+        <v>642258</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10">
       <c r="A142" s="1">
         <v>41518</v>
       </c>
@@ -3434,8 +3831,14 @@
       <c r="H142">
         <v>9</v>
       </c>
-    </row>
-    <row r="143" spans="1:8">
+      <c r="I142" s="2">
+        <v>270788</v>
+      </c>
+      <c r="J142" s="2">
+        <v>483518</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10">
       <c r="A143" s="1">
         <v>41548</v>
       </c>
@@ -3460,8 +3863,14 @@
       <c r="H143">
         <v>10</v>
       </c>
-    </row>
-    <row r="144" spans="1:8">
+      <c r="I143" s="2">
+        <v>221004</v>
+      </c>
+      <c r="J143" s="2">
+        <v>343273</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10">
       <c r="A144" s="1">
         <v>41579</v>
       </c>
@@ -3486,8 +3895,14 @@
       <c r="H144">
         <v>11</v>
       </c>
-    </row>
-    <row r="145" spans="1:8">
+      <c r="I144" s="2">
+        <v>236031</v>
+      </c>
+      <c r="J144" s="2">
+        <v>276428</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10">
       <c r="A145" s="1">
         <v>41609</v>
       </c>
@@ -3512,8 +3927,14 @@
       <c r="H145">
         <v>12</v>
       </c>
-    </row>
-    <row r="146" spans="1:8">
+      <c r="I145" s="2">
+        <v>240629</v>
+      </c>
+      <c r="J145" s="2">
+        <v>276234</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10">
       <c r="A146" s="1">
         <v>41640</v>
       </c>
@@ -3538,8 +3959,14 @@
       <c r="H146">
         <v>1</v>
       </c>
-    </row>
-    <row r="147" spans="1:8">
+      <c r="I146" s="2">
+        <v>268861</v>
+      </c>
+      <c r="J146" s="2">
+        <v>296708</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10">
       <c r="A147" s="1">
         <v>41671</v>
       </c>
@@ -3564,8 +3991,14 @@
       <c r="H147">
         <v>2</v>
       </c>
-    </row>
-    <row r="148" spans="1:8">
+      <c r="I147" s="2">
+        <v>305390</v>
+      </c>
+      <c r="J147" s="2">
+        <v>326295</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10">
       <c r="A148" s="1">
         <v>41699</v>
       </c>
@@ -3590,8 +4023,14 @@
       <c r="H148">
         <v>3</v>
       </c>
-    </row>
-    <row r="149" spans="1:8">
+      <c r="I148" s="2">
+        <v>361470</v>
+      </c>
+      <c r="J148" s="2">
+        <v>423768</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10">
       <c r="A149" s="1">
         <v>41730</v>
       </c>
@@ -3616,8 +4055,14 @@
       <c r="H149">
         <v>4</v>
       </c>
-    </row>
-    <row r="150" spans="1:8">
+      <c r="I149" s="2">
+        <v>377197</v>
+      </c>
+      <c r="J149" s="2">
+        <v>531947</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10">
       <c r="A150" s="1">
         <v>41760</v>
       </c>
@@ -3642,8 +4087,14 @@
       <c r="H150">
         <v>5</v>
       </c>
-    </row>
-    <row r="151" spans="1:8">
+      <c r="I150" s="2">
+        <v>333845</v>
+      </c>
+      <c r="J150" s="2">
+        <v>517031</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10">
       <c r="A151" s="1">
         <v>41791</v>
       </c>
@@ -3668,8 +4119,14 @@
       <c r="H151">
         <v>6</v>
       </c>
-    </row>
-    <row r="152" spans="1:8">
+      <c r="I151" s="2">
+        <v>315166</v>
+      </c>
+      <c r="J151" s="2">
+        <v>573852</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10">
       <c r="A152" s="1">
         <v>41821</v>
       </c>
@@ -3694,8 +4151,14 @@
       <c r="H152">
         <v>7</v>
       </c>
-    </row>
-    <row r="153" spans="1:8">
+      <c r="I152" s="2">
+        <v>343709</v>
+      </c>
+      <c r="J152" s="2">
+        <v>692053</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10">
       <c r="A153" s="1">
         <v>41852</v>
       </c>
@@ -3720,8 +4183,14 @@
       <c r="H153">
         <v>8</v>
       </c>
-    </row>
-    <row r="154" spans="1:8">
+      <c r="I153" s="2">
+        <v>312549</v>
+      </c>
+      <c r="J153" s="2">
+        <v>757683</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10">
       <c r="A154" s="1">
         <v>41883</v>
       </c>
@@ -3746,8 +4215,14 @@
       <c r="H154">
         <v>9</v>
       </c>
-    </row>
-    <row r="155" spans="1:8">
+      <c r="I154" s="2">
+        <v>341729</v>
+      </c>
+      <c r="J154" s="2">
+        <v>564078</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10">
       <c r="A155" s="1">
         <v>41913</v>
       </c>
@@ -3772,8 +4247,14 @@
       <c r="H155">
         <v>10</v>
       </c>
-    </row>
-    <row r="156" spans="1:8">
+      <c r="I155" s="2">
+        <v>347778</v>
+      </c>
+      <c r="J155" s="2">
+        <v>562278</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10">
       <c r="A156" s="1">
         <v>41944</v>
       </c>
@@ -3798,8 +4279,14 @@
       <c r="H156">
         <v>11</v>
       </c>
-    </row>
-    <row r="157" spans="1:8">
+      <c r="I156" s="2">
+        <v>332517</v>
+      </c>
+      <c r="J156" s="2">
+        <v>460671</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10">
       <c r="A157" s="1">
         <v>41974</v>
       </c>
@@ -3824,8 +4311,14 @@
       <c r="H157">
         <v>12</v>
       </c>
-    </row>
-    <row r="158" spans="1:8">
+      <c r="I157" s="2">
+        <v>346941</v>
+      </c>
+      <c r="J157" s="2">
+        <v>420501</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10">
       <c r="A158" s="1">
         <v>42005</v>
       </c>
@@ -3850,8 +4343,14 @@
       <c r="H158">
         <v>1</v>
       </c>
-    </row>
-    <row r="159" spans="1:8">
+      <c r="I158" s="2">
+        <v>321458</v>
+      </c>
+      <c r="J158" s="2">
+        <v>394345</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10">
       <c r="A159" s="1">
         <v>42036</v>
       </c>
@@ -3876,8 +4375,14 @@
       <c r="H159">
         <v>2</v>
       </c>
-    </row>
-    <row r="160" spans="1:8">
+      <c r="I159" s="2">
+        <v>406239</v>
+      </c>
+      <c r="J159" s="2">
+        <v>516787</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10">
       <c r="A160" s="1">
         <v>42064</v>
       </c>
@@ -3902,8 +4407,11 @@
       <c r="H160">
         <v>3</v>
       </c>
-    </row>
-    <row r="161" spans="1:8">
+      <c r="J160" s="5">
+        <v>515130</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10">
       <c r="A161" s="1">
         <v>42095</v>
       </c>
@@ -3928,8 +4436,11 @@
       <c r="H161">
         <v>4</v>
       </c>
-    </row>
-    <row r="162" spans="1:8">
+      <c r="J161" s="5">
+        <v>641610</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10">
       <c r="A162" s="1">
         <v>42125</v>
       </c>
@@ -3952,7 +4463,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:10">
       <c r="A163" s="1">
         <v>42156</v>
       </c>
@@ -3975,7 +4486,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:10">
       <c r="A164" s="1">
         <v>42186</v>
       </c>
@@ -3998,7 +4509,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:10">
       <c r="A165" s="1">
         <v>42217</v>
       </c>
@@ -4021,7 +4532,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:10">
       <c r="A166" s="1">
         <v>42248</v>
       </c>
@@ -4044,7 +4555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:10">
       <c r="A167" s="1">
         <v>42278</v>
       </c>
@@ -4067,7 +4578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:10">
       <c r="A168" s="1">
         <v>42309</v>
       </c>
@@ -4090,7 +4601,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:10">
       <c r="A169" s="1">
         <v>42339</v>
       </c>
@@ -4113,7 +4624,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:10">
       <c r="A170" s="1">
         <v>42370</v>
       </c>
@@ -4124,7 +4635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:10">
       <c r="A171" s="1">
         <v>42401</v>
       </c>
@@ -4135,7 +4646,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:10">
       <c r="A172" s="1">
         <v>42430</v>
       </c>
@@ -4146,7 +4657,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:10">
       <c r="A173" s="1">
         <v>42461</v>
       </c>
@@ -4157,7 +4668,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:10">
       <c r="A174" s="1">
         <v>42491</v>
       </c>
@@ -4168,7 +4679,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:10">
       <c r="A175" s="1">
         <v>42522</v>
       </c>
@@ -4179,7 +4690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:10">
       <c r="A176" s="1">
         <v>42552</v>
       </c>
@@ -4257,6 +4768,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="J2:L182">
+    <sortCondition ref="J2:J182"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>